<commit_message>
mise a jour des methodes delete de client identity claimobject et unité
</commit_message>
<xml_diff>
--- a/storage/app/public/excels/objects.xlsx
+++ b/storage/app/public/excels/objects.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">La description sur l’objet de plainte</t>
   </si>
   <si>
-    <t xml:space="preserve">le status du niveau de gravité</t>
+    <t xml:space="preserve">le status du niveau de gravité         Valeurs possibles :(low,medium,high)</t>
   </si>
   <si>
     <t xml:space="preserve">le nombre de jour pour la durée de traitement de la plainte</t>
@@ -178,10 +178,10 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G2"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.57"/>
@@ -189,7 +189,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="15.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="20"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="26"/>

</xml_diff>